<commit_message>
Coded the initial version for HA Data Extraction, started working on Data Exploration
</commit_message>
<xml_diff>
--- a/Data Frames/Analyzed/Weighted.xlsx
+++ b/Data Frames/Analyzed/Weighted.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AU451FE\OneDrive - EY\Desktop\Python\Hearthstone_Archmage\Data Frames\Analyzed\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_FFC65FC0344968C81C160B3293FADC61775433BA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF666A4B-9268-4260-B5B5-E7A6BB2E9518}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -187,8 +193,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +257,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -297,7 +311,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -329,9 +343,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -363,6 +395,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -538,14 +588,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -580,50 +638,50 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2">
-        <v>0.5790894941634241</v>
+        <v>0.57908949416342415</v>
       </c>
       <c r="C2">
-        <v>0.5985175097276264</v>
+        <v>0.59851750972762641</v>
       </c>
       <c r="D2">
-        <v>0.4745486381322956</v>
+        <v>0.47454863813229559</v>
       </c>
       <c r="E2">
         <v>0.4606420233463035</v>
       </c>
       <c r="F2">
-        <v>0.7019727626459142</v>
+        <v>0.70197276264591424</v>
       </c>
       <c r="G2">
-        <v>0.6930661478599222</v>
+        <v>0.69306614785992215</v>
       </c>
       <c r="H2">
-        <v>0.5724357976653696</v>
+        <v>0.57243579766536956</v>
       </c>
       <c r="I2">
         <v>0.627591439688716</v>
       </c>
       <c r="J2">
-        <v>0.5022529182879377</v>
+        <v>0.50225291828793772</v>
       </c>
       <c r="K2">
         <v>0.6661789883268483</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3">
-        <v>0.6023612273361227</v>
+        <v>0.60236122733612274</v>
       </c>
       <c r="C3">
-        <v>0.5842888578955525</v>
+        <v>0.58428885789555252</v>
       </c>
       <c r="D3">
         <v>0.454021850302185</v>
@@ -632,243 +690,243 @@
         <v>0.4927495738416241</v>
       </c>
       <c r="F3">
-        <v>0.6876785991011932</v>
+        <v>0.68767859910119322</v>
       </c>
       <c r="G3">
-        <v>0.6581915388191538</v>
+        <v>0.65819153881915382</v>
       </c>
       <c r="H3">
-        <v>0.6285699674569967</v>
+        <v>0.62856996745699667</v>
       </c>
       <c r="I3">
-        <v>0.6247999380133271</v>
+        <v>0.62479993801332712</v>
       </c>
       <c r="J3">
-        <v>0.5448495273516195</v>
+        <v>0.54484952735161951</v>
       </c>
       <c r="K3">
-        <v>0.8192135440880212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>0.81921354408802116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4">
-        <v>0.5472413793103448</v>
+        <v>0.54724137931034478</v>
       </c>
       <c r="C4">
-        <v>0.4720689655172414</v>
+        <v>0.47206896551724142</v>
       </c>
       <c r="D4">
-        <v>0.4946551724137931</v>
+        <v>0.49465517241379309</v>
       </c>
       <c r="E4">
-        <v>0.5531724137931034</v>
+        <v>0.55317241379310345</v>
       </c>
       <c r="F4">
-        <v>0.5887586206896551</v>
+        <v>0.58875862068965512</v>
       </c>
       <c r="G4">
-        <v>0.4696551724137931</v>
+        <v>0.46965517241379312</v>
       </c>
       <c r="H4">
-        <v>0.6442413793103449</v>
+        <v>0.64424137931034486</v>
       </c>
       <c r="I4">
-        <v>0.5748275862068964</v>
+        <v>0.57482758620689645</v>
       </c>
       <c r="J4">
-        <v>0.507448275862069</v>
+        <v>0.50744827586206898</v>
       </c>
       <c r="K4">
-        <v>0.6829655172413792</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>0.68296551724137922</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B5">
-        <v>0.4873897967317656</v>
+        <v>0.48738979673176558</v>
       </c>
       <c r="C5">
-        <v>0.4137353527301714</v>
+        <v>0.41373535273017142</v>
       </c>
       <c r="D5">
-        <v>0.4247122359505779</v>
+        <v>0.42471223595057789</v>
       </c>
       <c r="E5">
-        <v>0.5331725787166202</v>
+        <v>0.53317257871662016</v>
       </c>
       <c r="F5">
-        <v>0.5206062176165803</v>
+        <v>0.52060621761658032</v>
       </c>
       <c r="G5">
-        <v>0.327238341968912</v>
+        <v>0.32723834196891199</v>
       </c>
       <c r="H5">
         <v>0.5146990833001196</v>
       </c>
       <c r="I5">
-        <v>0.5339194898365882</v>
+        <v>0.53391948983658821</v>
       </c>
       <c r="J5">
-        <v>0.4794479872459148</v>
+        <v>0.47944798724591481</v>
       </c>
       <c r="K5">
-        <v>0.6105607811877242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>0.61056078118772417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6">
-        <v>0.5067793144918822</v>
+        <v>0.50677931449188218</v>
       </c>
       <c r="C6">
-        <v>0.4851960312687914</v>
+        <v>0.48519603126879141</v>
       </c>
       <c r="D6">
-        <v>0.4107239927841251</v>
+        <v>0.41072399278412508</v>
       </c>
       <c r="E6">
         <v>0.4617330126277811</v>
       </c>
       <c r="F6">
-        <v>0.5878496692723995</v>
+        <v>0.58784966927239946</v>
       </c>
       <c r="G6">
-        <v>0.4361828021647624</v>
+        <v>0.43618280216476241</v>
       </c>
       <c r="H6">
-        <v>0.5193908598917618</v>
+        <v>0.51939085989176181</v>
       </c>
       <c r="I6">
-        <v>0.531262778111846</v>
+        <v>0.53126277811184597</v>
       </c>
       <c r="J6">
-        <v>0.4465273601924233</v>
+        <v>0.44652736019242328</v>
       </c>
       <c r="K6">
-        <v>0.6265868911605532</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>0.62658689116055322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B7">
-        <v>0.5426153846153847</v>
+        <v>0.54261538461538472</v>
       </c>
       <c r="C7">
-        <v>0.5756307692307693</v>
+        <v>0.57563076923076928</v>
       </c>
       <c r="D7">
-        <v>0.3914461538461539</v>
+        <v>0.39144615384615389</v>
       </c>
       <c r="E7">
-        <v>0.4450307692307693</v>
+        <v>0.44503076923076929</v>
       </c>
       <c r="F7">
         <v>0.6954769230769231</v>
       </c>
       <c r="G7">
-        <v>0.6090769230769231</v>
+        <v>0.60907692307692307</v>
       </c>
       <c r="H7">
-        <v>0.4892615384615385</v>
+        <v>0.48926153846153853</v>
       </c>
       <c r="I7">
         <v>0.5815538461538462</v>
       </c>
       <c r="J7">
-        <v>0.4980153846153846</v>
+        <v>0.49801538461538458</v>
       </c>
       <c r="K7">
-        <v>0.6340615384615386</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>0.63406153846153857</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B8">
-        <v>0.4809704321455648</v>
+        <v>0.48097043214556479</v>
       </c>
       <c r="C8">
         <v>0.6072418498862775</v>
       </c>
       <c r="D8">
-        <v>0.3988271417740712</v>
+        <v>0.39882714177407119</v>
       </c>
       <c r="E8">
         <v>0.4666921910538287</v>
       </c>
       <c r="F8">
-        <v>0.5415238817285822</v>
+        <v>0.54152388172858223</v>
       </c>
       <c r="G8">
-        <v>0.467557240333586</v>
+        <v>0.46755724033358598</v>
       </c>
       <c r="H8">
         <v>0.3234518574677786</v>
       </c>
       <c r="I8">
-        <v>0.5190470053070507</v>
+        <v>0.51904700530705072</v>
       </c>
       <c r="J8">
-        <v>0.5150454890068233</v>
+        <v>0.51504548900682334</v>
       </c>
       <c r="K8">
-        <v>0.3626717210007581</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>0.36267172100075812</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B9">
-        <v>0.3666592039800995</v>
+        <v>0.36665920398009949</v>
       </c>
       <c r="C9">
-        <v>0.3619707711442786</v>
+        <v>0.36197077114427861</v>
       </c>
       <c r="D9">
         <v>0.2490217661691542</v>
       </c>
       <c r="E9">
-        <v>0.27631592039801</v>
+        <v>0.27631592039801001</v>
       </c>
       <c r="F9">
-        <v>0.5312294776119402</v>
+        <v>0.53122947761194017</v>
       </c>
       <c r="G9">
-        <v>0.293172263681592</v>
+        <v>0.29317226368159199</v>
       </c>
       <c r="H9">
-        <v>0.4481473880597014</v>
+        <v>0.44814738805970139</v>
       </c>
       <c r="I9">
-        <v>0.4391299751243781</v>
+        <v>0.43912997512437812</v>
       </c>
       <c r="J9">
-        <v>0.2566511194029851</v>
+        <v>0.25665111940298507</v>
       </c>
       <c r="K9">
         <v>0.4418289800995025</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10">
-        <v>0.3862290950744559</v>
+        <v>0.38622909507445591</v>
       </c>
       <c r="C10">
-        <v>0.5648820160366552</v>
+        <v>0.56488201603665522</v>
       </c>
       <c r="D10">
         <v>0.427610538373425</v>
@@ -877,165 +935,165 @@
         <v>0.3929450171821306</v>
       </c>
       <c r="F10">
-        <v>0.3539965635738831</v>
+        <v>0.35399656357388309</v>
       </c>
       <c r="G10">
-        <v>0.3887823596792669</v>
+        <v>0.38878235967926689</v>
       </c>
       <c r="H10">
-        <v>0.3192703321878579</v>
+        <v>0.31927033218785789</v>
       </c>
       <c r="I10">
-        <v>0.4413081328751431</v>
+        <v>0.44130813287514309</v>
       </c>
       <c r="J10">
-        <v>0.3331122565864834</v>
+        <v>0.33311225658648341</v>
       </c>
       <c r="K10">
-        <v>0.3582142038946163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>0.35821420389461628</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B11">
-        <v>0.5668496158068058</v>
+        <v>0.56684961580680582</v>
       </c>
       <c r="C11">
-        <v>0.6639936333699232</v>
+        <v>0.66399363336992323</v>
       </c>
       <c r="D11">
-        <v>0.5181163556531285</v>
+        <v>0.51811635565312852</v>
       </c>
       <c r="E11">
-        <v>0.3952305159165752</v>
+        <v>0.39523051591657521</v>
       </c>
       <c r="F11">
-        <v>0.6164109769484082</v>
+        <v>0.61641097694840818</v>
       </c>
       <c r="G11">
-        <v>0.5827828759604831</v>
+        <v>0.58278287596048306</v>
       </c>
       <c r="H11">
-        <v>0.5994472008781558</v>
+        <v>0.59944720087815584</v>
       </c>
       <c r="I11">
-        <v>0.5832897914379803</v>
+        <v>0.58328979143798032</v>
       </c>
       <c r="J11">
-        <v>0.48908144895719</v>
+        <v>0.48908144895719002</v>
       </c>
       <c r="K11">
-        <v>0.6331216245883645</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>0.63312162458836452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B12">
-        <v>0.579822489880541</v>
+        <v>0.57982248988054097</v>
       </c>
       <c r="C12">
         <v>0.6445642215421068</v>
       </c>
       <c r="D12">
-        <v>0.6215891006022313</v>
+        <v>0.62158910060223127</v>
       </c>
       <c r="E12">
-        <v>0.5853377431138316</v>
+        <v>0.58533774311383158</v>
       </c>
       <c r="F12">
-        <v>0.6291472011057361</v>
+        <v>0.62914720110573608</v>
       </c>
       <c r="G12">
-        <v>0.6039343469246716</v>
+        <v>0.60393434692467163</v>
       </c>
       <c r="H12">
-        <v>0.5419512291440418</v>
+        <v>0.54195122914404181</v>
       </c>
       <c r="I12">
-        <v>0.6480553855267054</v>
+        <v>0.64805538552670539</v>
       </c>
       <c r="J12">
-        <v>0.505948366077599</v>
+        <v>0.50594836607759897</v>
       </c>
       <c r="K12">
-        <v>0.5865024187975121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>0.58650241879751208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B13">
-        <v>0.6077457520453114</v>
+        <v>0.60774575204531145</v>
       </c>
       <c r="C13">
-        <v>0.6182699811202015</v>
+        <v>0.61826998112020148</v>
       </c>
       <c r="D13">
-        <v>0.6284820641913152</v>
+        <v>0.62848206419131525</v>
       </c>
       <c r="E13">
-        <v>0.5763303964757709</v>
+        <v>0.57633039647577089</v>
       </c>
       <c r="F13">
-        <v>0.7345613593455003</v>
+        <v>0.73456135934550026</v>
       </c>
       <c r="G13">
-        <v>0.6085789804908748</v>
+        <v>0.60857898049087478</v>
       </c>
       <c r="H13">
-        <v>0.4834883574575204</v>
+        <v>0.48348835745752039</v>
       </c>
       <c r="I13">
-        <v>0.6782762743864065</v>
+        <v>0.67827627438640647</v>
       </c>
       <c r="J13">
-        <v>0.5638565135305222</v>
+        <v>0.56385651353052224</v>
       </c>
       <c r="K13">
         <v>0.686074260541221</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B14">
-        <v>0.4991318327974277</v>
+        <v>0.49913183279742768</v>
       </c>
       <c r="C14">
-        <v>0.4929983922829582</v>
+        <v>0.49299839228295822</v>
       </c>
       <c r="D14">
-        <v>0.3849895498392283</v>
+        <v>0.38498954983922828</v>
       </c>
       <c r="E14">
-        <v>0.4222789389067524</v>
+        <v>0.42227893890675239</v>
       </c>
       <c r="F14">
-        <v>0.5126832797427653</v>
+        <v>0.51268327974276529</v>
       </c>
       <c r="G14">
-        <v>0.5779734726688104</v>
+        <v>0.57797347266881038</v>
       </c>
       <c r="H14">
-        <v>0.5733094855305466</v>
+        <v>0.57330948553054661</v>
       </c>
       <c r="I14">
-        <v>0.5051254019292605</v>
+        <v>0.50512540192926048</v>
       </c>
       <c r="J14">
-        <v>0.4562516077170418</v>
+        <v>0.45625160771704182</v>
       </c>
       <c r="K14">
-        <v>0.6242033762057879</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>0.62420337620578792</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1043,354 +1101,354 @@
         <v>0.496</v>
       </c>
       <c r="C15">
-        <v>0.466</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="D15">
-        <v>0.479</v>
+        <v>0.47899999999999998</v>
       </c>
       <c r="E15">
         <v>0.379</v>
       </c>
       <c r="F15">
-        <v>0.491</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="G15">
-        <v>0.547</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="H15">
-        <v>0.604</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="I15">
-        <v>0.462</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="J15">
-        <v>0.456</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="K15">
-        <v>0.602</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B16">
-        <v>0.4385107033639143</v>
+        <v>0.43851070336391429</v>
       </c>
       <c r="C16">
-        <v>0.4188695208970439</v>
+        <v>0.41886952089704388</v>
       </c>
       <c r="D16">
-        <v>0.4950275229357798</v>
+        <v>0.49502752293577978</v>
       </c>
       <c r="E16">
-        <v>0.3403323139653415</v>
+        <v>0.34033231396534153</v>
       </c>
       <c r="F16">
-        <v>0.3835188583078492</v>
+        <v>0.38351885830784921</v>
       </c>
       <c r="G16">
         <v>0.5684556574923546</v>
       </c>
       <c r="H16">
-        <v>0.5543975535168195</v>
+        <v>0.55439755351681952</v>
       </c>
       <c r="I16">
-        <v>0.5397706422018348</v>
+        <v>0.53977064220183479</v>
       </c>
       <c r="J16">
-        <v>0.3820305810397553</v>
+        <v>0.38203058103975529</v>
       </c>
       <c r="K16">
-        <v>0.4313465851172273</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>0.43134658511722729</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B17">
-        <v>0.5421805194805195</v>
+        <v>0.54218051948051948</v>
       </c>
       <c r="C17">
-        <v>0.5096207792207791</v>
+        <v>0.50962077922077909</v>
       </c>
       <c r="D17">
-        <v>0.5045837662337662</v>
+        <v>0.50458376623376622</v>
       </c>
       <c r="E17">
-        <v>0.427164935064935</v>
+        <v>0.42716493506493503</v>
       </c>
       <c r="F17">
-        <v>0.6103116883116882</v>
+        <v>0.61031168831168825</v>
       </c>
       <c r="G17">
-        <v>0.5246935064935064</v>
+        <v>0.52469350649350643</v>
       </c>
       <c r="H17">
-        <v>0.652283766233766</v>
+        <v>0.65228376623376605</v>
       </c>
       <c r="I17">
-        <v>0.5749642857142857</v>
+        <v>0.57496428571428571</v>
       </c>
       <c r="J17">
-        <v>0.451861038961039</v>
+        <v>0.45186103896103902</v>
       </c>
       <c r="K17">
-        <v>0.6457155844155844</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>0.64571558441558441</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B18">
-        <v>0.449024861878453</v>
+        <v>0.44902486187845297</v>
       </c>
       <c r="C18">
-        <v>0.3969576427255985</v>
+        <v>0.39695764272559853</v>
       </c>
       <c r="D18">
-        <v>0.4533802946593002</v>
+        <v>0.45338029465930019</v>
       </c>
       <c r="E18">
-        <v>0.3814493554327809</v>
+        <v>0.38144935543278091</v>
       </c>
       <c r="F18">
         <v>0.4698370165745856</v>
       </c>
       <c r="G18">
-        <v>0.5157817679558011</v>
+        <v>0.51578176795580111</v>
       </c>
       <c r="H18">
-        <v>0.5556049723756905</v>
+        <v>0.55560497237569051</v>
       </c>
       <c r="I18">
-        <v>0.4894742173112339</v>
+        <v>0.48947421731123392</v>
       </c>
       <c r="J18">
-        <v>0.3135220994475139</v>
+        <v>0.31352209944751391</v>
       </c>
       <c r="K18">
-        <v>0.525023020257827</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>0.52502302025782699</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B19">
-        <v>0.4490887818306951</v>
+        <v>0.44908878183069512</v>
       </c>
       <c r="C19">
-        <v>0.4255299380591879</v>
+        <v>0.42552993805918787</v>
       </c>
       <c r="D19">
-        <v>0.5103854094975913</v>
+        <v>0.51038540949759126</v>
       </c>
       <c r="E19">
-        <v>0.3904459738472127</v>
+        <v>0.39044597384721269</v>
       </c>
       <c r="F19">
-        <v>0.4708967653131452</v>
+        <v>0.47089676531314523</v>
       </c>
       <c r="G19">
-        <v>0.4766207845836201</v>
+        <v>0.47662078458362012</v>
       </c>
       <c r="H19">
-        <v>0.5216841018582244</v>
+        <v>0.52168410185822445</v>
       </c>
       <c r="I19">
-        <v>0.5062278045423262</v>
+        <v>0.50622780454232619</v>
       </c>
       <c r="J19">
-        <v>0.3480123881624225</v>
+        <v>0.34801238816242253</v>
       </c>
       <c r="K19">
-        <v>0.4973434273916035</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>0.49734342739160348</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B20">
-        <v>0.4305869311551926</v>
+        <v>0.43058693115519259</v>
       </c>
       <c r="C20">
-        <v>0.5136907817969661</v>
+        <v>0.51369078179696614</v>
       </c>
       <c r="D20">
-        <v>0.463458576429405</v>
+        <v>0.46345857642940502</v>
       </c>
       <c r="E20">
-        <v>0.4181843640606768</v>
+        <v>0.41818436406067683</v>
       </c>
       <c r="F20">
         <v>0.431463243873979</v>
       </c>
       <c r="G20">
-        <v>0.4396779463243874</v>
+        <v>0.43967794632438739</v>
       </c>
       <c r="H20">
-        <v>0.3805344224037339</v>
+        <v>0.38053442240373392</v>
       </c>
       <c r="I20">
-        <v>0.4423138856476079</v>
+        <v>0.44231388564760787</v>
       </c>
       <c r="J20">
-        <v>0.3880373395565928</v>
+        <v>0.38803733955659281</v>
       </c>
       <c r="K20">
-        <v>0.4489848308051342</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>0.44898483080513418</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B21">
-        <v>0.5695035971223023</v>
+        <v>0.56950359712230225</v>
       </c>
       <c r="C21">
-        <v>0.4962800221361373</v>
+        <v>0.49628002213613731</v>
       </c>
       <c r="D21">
-        <v>0.5592263420033206</v>
+        <v>0.55922634200332055</v>
       </c>
       <c r="E21">
-        <v>0.4592988378527946</v>
+        <v>0.45929883785279457</v>
       </c>
       <c r="F21">
-        <v>0.6859513004980632</v>
+        <v>0.68595130049806319</v>
       </c>
       <c r="G21">
-        <v>0.5978483674598782</v>
+        <v>0.59784836745987824</v>
       </c>
       <c r="H21">
-        <v>0.6909302711676811</v>
+        <v>0.69093027116768113</v>
       </c>
       <c r="I21">
-        <v>0.5800979524073049</v>
+        <v>0.58009795240730488</v>
       </c>
       <c r="J21">
-        <v>0.4520990592141672</v>
+        <v>0.45209905921416721</v>
       </c>
       <c r="K21">
-        <v>0.656650249031544</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>0.65665024903154401</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B22">
-        <v>0.5317954545454546</v>
+        <v>0.53179545454545463</v>
       </c>
       <c r="C22">
-        <v>0.5596590909090909</v>
+        <v>0.55965909090909094</v>
       </c>
       <c r="D22">
-        <v>0.5244545454545455</v>
+        <v>0.52445454545454551</v>
       </c>
       <c r="E22">
-        <v>0.5381818181818182</v>
+        <v>0.53818181818181821</v>
       </c>
       <c r="F22">
-        <v>0.5888295454545455</v>
+        <v>0.58882954545454547</v>
       </c>
       <c r="G22">
-        <v>0.5519886363636364</v>
+        <v>0.55198863636363638</v>
       </c>
       <c r="H22">
-        <v>0.5074204545454546</v>
+        <v>0.50742045454545459</v>
       </c>
       <c r="I22">
         <v>0.548534090909091</v>
       </c>
       <c r="J22">
-        <v>0.4819204545454546</v>
+        <v>0.48192045454545462</v>
       </c>
       <c r="K22">
-        <v>0.5317613636363636</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>0.53176136363636362</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B23">
-        <v>0.5680675977653631</v>
+        <v>0.56806759776536309</v>
       </c>
       <c r="C23">
-        <v>0.5713648044692737</v>
+        <v>0.57136480446927373</v>
       </c>
       <c r="D23">
-        <v>0.5134418994413408</v>
+        <v>0.51344189944134078</v>
       </c>
       <c r="E23">
-        <v>0.6394642458100558</v>
+        <v>0.63946424581005579</v>
       </c>
       <c r="F23">
         <v>0.6456597765363129</v>
       </c>
       <c r="G23">
-        <v>0.571999441340782</v>
+        <v>0.57199944134078196</v>
       </c>
       <c r="H23">
-        <v>0.504986592178771</v>
+        <v>0.50498659217877095</v>
       </c>
       <c r="I23">
-        <v>0.6194960893854748</v>
+        <v>0.61949608938547485</v>
       </c>
       <c r="J23">
-        <v>0.5552307262569831</v>
+        <v>0.55523072625698311</v>
       </c>
       <c r="K23">
-        <v>0.4715877094972067</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>0.47158770949720669</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B24">
-        <v>0.5709780033840947</v>
+        <v>0.57097800338409466</v>
       </c>
       <c r="C24">
-        <v>0.5170879864636211</v>
+        <v>0.51708798646362109</v>
       </c>
       <c r="D24">
-        <v>0.5910659898477156</v>
+        <v>0.59106598984771563</v>
       </c>
       <c r="E24">
-        <v>0.539585448392555</v>
+        <v>0.53958544839255496</v>
       </c>
       <c r="F24">
-        <v>0.6900028200789622</v>
+        <v>0.69000282007896219</v>
       </c>
       <c r="G24">
-        <v>0.5826226734348562</v>
+        <v>0.58262267343485619</v>
       </c>
       <c r="H24">
-        <v>0.5800310208685843</v>
+        <v>0.58003102086858427</v>
       </c>
       <c r="I24">
-        <v>0.6051816130851665</v>
+        <v>0.60518161308516649</v>
       </c>
       <c r="J24">
-        <v>0.4547354765933446</v>
+        <v>0.45473547659334462</v>
       </c>
       <c r="K24">
-        <v>0.6014371122391426</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>0.60143711223914265</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B25">
-        <v>0.463</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="C25">
         <v>0.41</v>
@@ -1399,28 +1457,28 @@
         <v>0.5</v>
       </c>
       <c r="E25">
-        <v>0.403</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="F25">
         <v>0.495</v>
       </c>
       <c r="G25">
-        <v>0.517</v>
+        <v>0.51700000000000002</v>
       </c>
       <c r="H25">
-        <v>0.706</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="I25">
-        <v>0.5600000000000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="J25">
-        <v>0.263</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="K25">
         <v>0.48</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -1428,209 +1486,209 @@
         <v>0.4914627737226277</v>
       </c>
       <c r="C26">
-        <v>0.5055182481751824</v>
+        <v>0.50551824817518243</v>
       </c>
       <c r="D26">
-        <v>0.5569343065693431</v>
+        <v>0.55693430656934306</v>
       </c>
       <c r="E26">
-        <v>0.6165693430656934</v>
+        <v>0.61656934306569344</v>
       </c>
       <c r="F26">
-        <v>0.4704554744525548</v>
+        <v>0.47045547445255481</v>
       </c>
       <c r="G26">
-        <v>0.5315255474452554</v>
+        <v>0.53152554744525538</v>
       </c>
       <c r="H26">
-        <v>0.4658759124087591</v>
+        <v>0.46587591240875909</v>
       </c>
       <c r="I26">
-        <v>0.5195518248175183</v>
+        <v>0.51955182481751827</v>
       </c>
       <c r="J26">
-        <v>0.4854379562043796</v>
+        <v>0.48543795620437957</v>
       </c>
       <c r="K26">
-        <v>0.2895109489051095</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>0.28951094890510948</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B27">
-        <v>0.4571888297872341</v>
+        <v>0.45718882978723407</v>
       </c>
       <c r="C27">
-        <v>0.4649281914893618</v>
+        <v>0.46492819148936182</v>
       </c>
       <c r="D27">
-        <v>0.4085851063829787</v>
+        <v>0.40858510638297868</v>
       </c>
       <c r="E27">
-        <v>0.5055079787234042</v>
+        <v>0.50550797872340425</v>
       </c>
       <c r="F27">
-        <v>0.4196622340425532</v>
+        <v>0.41966223404255321</v>
       </c>
       <c r="G27">
-        <v>0.4757712765957448</v>
+        <v>0.47577127659574481</v>
       </c>
       <c r="H27">
-        <v>0.4939308510638298</v>
+        <v>0.49393085106382978</v>
       </c>
       <c r="I27">
-        <v>0.5159920212765958</v>
+        <v>0.51599202127659582</v>
       </c>
       <c r="J27">
-        <v>0.4309335106382978</v>
+        <v>0.43093351063829782</v>
       </c>
       <c r="K27">
-        <v>0.388715425531915</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>0.38871542553191502</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B28">
-        <v>0.5130717557251908</v>
+        <v>0.51307175572519081</v>
       </c>
       <c r="C28">
-        <v>0.5135557251908398</v>
+        <v>0.51355572519083981</v>
       </c>
       <c r="D28">
-        <v>0.5573236641221375</v>
+        <v>0.55732366412213752</v>
       </c>
       <c r="E28">
-        <v>0.5996870229007634</v>
+        <v>0.59968702290076337</v>
       </c>
       <c r="F28">
-        <v>0.4445221374045802</v>
+        <v>0.44452213740458019</v>
       </c>
       <c r="G28">
-        <v>0.5441770992366413</v>
+        <v>0.54417709923664126</v>
       </c>
       <c r="H28">
-        <v>0.532514503816794</v>
+        <v>0.53251450381679399</v>
       </c>
       <c r="I28">
-        <v>0.5574290076335878</v>
+        <v>0.55742900763358783</v>
       </c>
       <c r="J28">
-        <v>0.4712</v>
+        <v>0.47120000000000001</v>
       </c>
       <c r="K28">
-        <v>0.3743022900763359</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>0.37430229007633592</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B29">
-        <v>0.4221092024539878</v>
+        <v>0.42210920245398781</v>
       </c>
       <c r="C29">
-        <v>0.4168822085889571</v>
+        <v>0.41688220858895708</v>
       </c>
       <c r="D29">
-        <v>0.4644061349693251</v>
+        <v>0.46440613496932509</v>
       </c>
       <c r="E29">
-        <v>0.475477300613497</v>
+        <v>0.47547730061349702</v>
       </c>
       <c r="F29">
-        <v>0.4054319018404908</v>
+        <v>0.40543190184049083</v>
       </c>
       <c r="G29">
-        <v>0.4464110429447853</v>
+        <v>0.44641104294478529</v>
       </c>
       <c r="H29">
-        <v>0.4432993865030675</v>
+        <v>0.44329938650306749</v>
       </c>
       <c r="I29">
-        <v>0.4494625766871166</v>
+        <v>0.44946257668711659</v>
       </c>
       <c r="J29">
-        <v>0.3820588957055214</v>
+        <v>0.38205889570552137</v>
       </c>
       <c r="K29">
-        <v>0.317719018404908</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>0.31771901840490802</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B30">
-        <v>0.4662355858648481</v>
+        <v>0.46623558586484809</v>
       </c>
       <c r="C30">
-        <v>0.5478704277743336</v>
+        <v>0.54787042777433359</v>
       </c>
       <c r="D30">
-        <v>0.5230700557966521</v>
+        <v>0.52307005579665211</v>
       </c>
       <c r="E30">
-        <v>0.5382777433353998</v>
+        <v>0.53827774333539979</v>
       </c>
       <c r="F30">
-        <v>0.3966367017978921</v>
+        <v>0.39663670179789212</v>
       </c>
       <c r="G30">
-        <v>0.4945114693118413</v>
+        <v>0.49451146931184131</v>
       </c>
       <c r="H30">
-        <v>0.5162603843769373</v>
+        <v>0.51626038437693733</v>
       </c>
       <c r="I30">
-        <v>0.4796670799752015</v>
+        <v>0.47966707997520153</v>
       </c>
       <c r="J30">
         <v>0.4119032858028519</v>
       </c>
       <c r="K30">
-        <v>0.3035275883446993</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>0.30352758834469928</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B31">
-        <v>0.5180593031875464</v>
+        <v>0.51805930318754645</v>
       </c>
       <c r="C31">
-        <v>0.5047299234000494</v>
+        <v>0.50472992340004941</v>
       </c>
       <c r="D31">
-        <v>0.5403575488015813</v>
+        <v>0.54035754880158127</v>
       </c>
       <c r="E31">
-        <v>0.4868178897949098</v>
+        <v>0.48681788979490981</v>
       </c>
       <c r="F31">
-        <v>0.5868851000741291</v>
+        <v>0.58688510007412908</v>
       </c>
       <c r="G31">
-        <v>0.5633298739807265</v>
+        <v>0.56332987398072654</v>
       </c>
       <c r="H31">
-        <v>0.4896725969854213</v>
+        <v>0.48967259698542132</v>
       </c>
       <c r="I31">
-        <v>0.5705347170743761</v>
+        <v>0.57053471707437609</v>
       </c>
       <c r="J31">
-        <v>0.49215468248085</v>
+        <v>0.49215468248084998</v>
       </c>
       <c r="K31">
-        <v>0.5750140845070423</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
+        <v>0.57501408450704228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -1638,69 +1696,69 @@
         <v>0.3678688524590164</v>
       </c>
       <c r="C32">
-        <v>0.4058196721311476</v>
+        <v>0.40581967213114761</v>
       </c>
       <c r="D32">
-        <v>0.32924043715847</v>
+        <v>0.32924043715847001</v>
       </c>
       <c r="E32">
         <v>0.2654918032786886</v>
       </c>
       <c r="F32">
-        <v>0.4265027322404372</v>
+        <v>0.42650273224043722</v>
       </c>
       <c r="G32">
-        <v>0.2742459016393443</v>
+        <v>0.27424590163934431</v>
       </c>
       <c r="H32">
-        <v>0.3489672131147541</v>
+        <v>0.34896721311475409</v>
       </c>
       <c r="I32">
-        <v>0.4898087431693989</v>
+        <v>0.48980874316939887</v>
       </c>
       <c r="J32">
-        <v>0.2842021857923497</v>
+        <v>0.28420218579234968</v>
       </c>
       <c r="K32">
-        <v>0.4689781420765028</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>0.46897814207650279</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B33">
-        <v>0.505208722741433</v>
+        <v>0.50520872274143303</v>
       </c>
       <c r="C33">
-        <v>0.5176292834890965</v>
+        <v>0.51762928348909654</v>
       </c>
       <c r="D33">
-        <v>0.3729231568016614</v>
+        <v>0.37292315680166138</v>
       </c>
       <c r="E33">
-        <v>0.336441329179647</v>
+        <v>0.33644132917964698</v>
       </c>
       <c r="F33">
-        <v>0.6619885773624091</v>
+        <v>0.66198857736240913</v>
       </c>
       <c r="G33">
-        <v>0.3203717549325026</v>
+        <v>0.32037175493250258</v>
       </c>
       <c r="H33">
-        <v>0.5242128764278297</v>
+        <v>0.52421287642782965</v>
       </c>
       <c r="I33">
-        <v>0.5890674974039459</v>
+        <v>0.58906749740394593</v>
       </c>
       <c r="J33">
-        <v>0.4335939771547248</v>
+        <v>0.43359397715472481</v>
       </c>
       <c r="K33">
-        <v>0.7366292834890965</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>0.73662928348909651</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
@@ -1708,39 +1766,39 @@
         <v>0.5518393124065768</v>
       </c>
       <c r="C34">
-        <v>0.5764656203288491</v>
+        <v>0.57646562032884907</v>
       </c>
       <c r="D34">
-        <v>0.4782369207772795</v>
+        <v>0.47823692077727947</v>
       </c>
       <c r="E34">
-        <v>0.4796823617339313</v>
+        <v>0.47968236173393131</v>
       </c>
       <c r="F34">
-        <v>0.5728273542600897</v>
+        <v>0.57282735426008968</v>
       </c>
       <c r="G34">
-        <v>0.6658647234678624</v>
+        <v>0.66586472346786241</v>
       </c>
       <c r="H34">
         <v>0.6575889387144993</v>
       </c>
       <c r="I34">
-        <v>0.5296711509715993</v>
+        <v>0.52967115097159934</v>
       </c>
       <c r="J34">
-        <v>0.4600859491778775</v>
+        <v>0.46008594917787748</v>
       </c>
       <c r="K34">
-        <v>0.6123393124065771</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>0.61233931240657713</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B35">
-        <v>0.6077886509917246</v>
+        <v>0.60778865099172463</v>
       </c>
       <c r="C35">
         <v>0.5560484697228425</v>
@@ -1749,133 +1807,133 @@
         <v>0.5540274530408511</v>
       </c>
       <c r="E35">
-        <v>0.5097950873505845</v>
+        <v>0.50979508735058454</v>
       </c>
       <c r="F35">
-        <v>0.7358781032444502</v>
+        <v>0.73587810324445024</v>
       </c>
       <c r="G35">
-        <v>0.5441356889531065</v>
+        <v>0.54413568895310649</v>
       </c>
       <c r="H35">
-        <v>0.6493777748587941</v>
+        <v>0.64937777485879411</v>
       </c>
       <c r="I35">
-        <v>0.655602522001839</v>
+        <v>0.65560252200183899</v>
       </c>
       <c r="J35">
-        <v>0.5463702876658348</v>
+        <v>0.54637028766583484</v>
       </c>
       <c r="K35">
-        <v>0.7896793642453697</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>0.78967936424536966</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B36">
-        <v>0.5921999999999999</v>
+        <v>0.59219999999999995</v>
       </c>
       <c r="C36">
-        <v>0.5362</v>
+        <v>0.53620000000000001</v>
       </c>
       <c r="D36">
-        <v>0.5564</v>
+        <v>0.55640000000000001</v>
       </c>
       <c r="E36">
-        <v>0.4833999999999999</v>
+        <v>0.48339999999999989</v>
       </c>
       <c r="F36">
-        <v>0.7364000000000002</v>
+        <v>0.73640000000000017</v>
       </c>
       <c r="G36">
-        <v>0.5327999999999999</v>
+        <v>0.53279999999999994</v>
       </c>
       <c r="H36">
-        <v>0.661</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="I36">
-        <v>0.6314</v>
+        <v>0.63139999999999996</v>
       </c>
       <c r="J36">
-        <v>0.5045999999999999</v>
+        <v>0.50459999999999994</v>
       </c>
       <c r="K36">
-        <v>0.8078</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
+        <v>0.80779999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B37">
-        <v>0.6205378086419753</v>
+        <v>0.62053780864197527</v>
       </c>
       <c r="C37">
-        <v>0.6067476851851852</v>
+        <v>0.60674768518518518</v>
       </c>
       <c r="D37">
-        <v>0.6158495370370369</v>
+        <v>0.61584953703703693</v>
       </c>
       <c r="E37">
-        <v>0.5939290123456791</v>
+        <v>0.59392901234567907</v>
       </c>
       <c r="F37">
-        <v>0.7023707561728396</v>
+        <v>0.70237075617283962</v>
       </c>
       <c r="G37">
-        <v>0.696770061728395</v>
+        <v>0.69677006172839495</v>
       </c>
       <c r="H37">
-        <v>0.6115625</v>
+        <v>0.61156250000000001</v>
       </c>
       <c r="I37">
-        <v>0.6763807870370371</v>
+        <v>0.67638078703703708</v>
       </c>
       <c r="J37">
-        <v>0.5727561728395061</v>
+        <v>0.57275617283950608</v>
       </c>
       <c r="K37">
-        <v>0.6579795524691356</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+        <v>0.65797955246913564</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B38">
-        <v>0.5457459505541347</v>
+        <v>0.54574595055413466</v>
       </c>
       <c r="C38">
-        <v>0.4776308610400682</v>
+        <v>0.47763086104006819</v>
       </c>
       <c r="D38">
-        <v>0.571916453537937</v>
+        <v>0.57191645353793696</v>
       </c>
       <c r="E38">
-        <v>0.4367894288150043</v>
+        <v>0.43678942881500432</v>
       </c>
       <c r="F38">
-        <v>0.6576479113384485</v>
+        <v>0.65764791133844847</v>
       </c>
       <c r="G38">
-        <v>0.5086513213981245</v>
+        <v>0.50865132139812452</v>
       </c>
       <c r="H38">
-        <v>0.5759283887468031</v>
+        <v>0.57592838874680308</v>
       </c>
       <c r="I38">
-        <v>0.6275055413469737</v>
+        <v>0.62750554134697367</v>
       </c>
       <c r="J38">
-        <v>0.4802779198635976</v>
+        <v>0.48027791986359758</v>
       </c>
       <c r="K38">
-        <v>0.655306905370844</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
+        <v>0.65530690537084402</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
@@ -1883,252 +1941,252 @@
         <v>0.5323201238390094</v>
       </c>
       <c r="C39">
-        <v>0.3802913312693498</v>
+        <v>0.38029133126934977</v>
       </c>
       <c r="D39">
         <v>0.5551306501547989</v>
       </c>
       <c r="E39">
-        <v>0.4470594427244582</v>
+        <v>0.44705944272445819</v>
       </c>
       <c r="F39">
-        <v>0.5546501547987616</v>
+        <v>0.55465015479876156</v>
       </c>
       <c r="G39">
-        <v>0.6363470588235294</v>
+        <v>0.63634705882352938</v>
       </c>
       <c r="H39">
         <v>0.7291582043343654</v>
       </c>
       <c r="I39">
-        <v>0.548256346749226</v>
+        <v>0.54825634674922596</v>
       </c>
       <c r="J39">
-        <v>0.4213770897832818</v>
+        <v>0.42137708978328181</v>
       </c>
       <c r="K39">
-        <v>0.5116448916408669</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+        <v>0.51164489164086691</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B40">
-        <v>0.462014598540146</v>
+        <v>0.46201459854014598</v>
       </c>
       <c r="C40">
-        <v>0.3352291970802919</v>
+        <v>0.33522919708029192</v>
       </c>
       <c r="D40">
-        <v>0.4903401459854015</v>
+        <v>0.49034014598540149</v>
       </c>
       <c r="E40">
-        <v>0.4902087591240876</v>
+        <v>0.49020875912408762</v>
       </c>
       <c r="F40">
-        <v>0.4372131386861314</v>
+        <v>0.43721313868613138</v>
       </c>
       <c r="G40">
-        <v>0.4937109489051095</v>
+        <v>0.49371094890510953</v>
       </c>
       <c r="H40">
         <v>0.5297021897810219</v>
       </c>
       <c r="I40">
-        <v>0.4914715328467154</v>
+        <v>0.49147153284671541</v>
       </c>
       <c r="J40">
-        <v>0.4526102189781022</v>
+        <v>0.45261021897810222</v>
       </c>
       <c r="K40">
-        <v>0.4240613138686132</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+        <v>0.42406131386861318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B41">
-        <v>0.416327763496144</v>
+        <v>0.41632776349614398</v>
       </c>
       <c r="C41">
         <v>0.2820167095115681</v>
       </c>
       <c r="D41">
-        <v>0.3849113110539845</v>
+        <v>0.38491131105398452</v>
       </c>
       <c r="E41">
-        <v>0.3955359897172236</v>
+        <v>0.39553598971722359</v>
       </c>
       <c r="F41">
-        <v>0.4152185089974293</v>
+        <v>0.41521850899742929</v>
       </c>
       <c r="G41">
-        <v>0.4487840616966581</v>
+        <v>0.44878406169665808</v>
       </c>
       <c r="H41">
-        <v>0.5584858611825193</v>
+        <v>0.55848586118251931</v>
       </c>
       <c r="I41">
-        <v>0.448159383033419</v>
+        <v>0.44815938303341901</v>
       </c>
       <c r="J41">
-        <v>0.3369370179948586</v>
+        <v>0.33693701799485859</v>
       </c>
       <c r="K41">
-        <v>0.4305565552699229</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
+        <v>0.43055655526992292</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B42">
-        <v>0.5047661870503596</v>
+        <v>0.50476618705035958</v>
       </c>
       <c r="C42">
-        <v>0.5186942446043166</v>
+        <v>0.51869424460431657</v>
       </c>
       <c r="D42">
-        <v>0.6136942446043164</v>
+        <v>0.61369424460431643</v>
       </c>
       <c r="E42">
-        <v>0.4365665467625899</v>
+        <v>0.43656654676258988</v>
       </c>
       <c r="F42">
-        <v>0.5549856115107913</v>
+        <v>0.55498561151079129</v>
       </c>
       <c r="G42">
-        <v>0.5590395683453238</v>
+        <v>0.55903956834532376</v>
       </c>
       <c r="H42">
         <v>0.5438129496402877</v>
       </c>
       <c r="I42">
-        <v>0.597861510791367</v>
+        <v>0.59786151079136696</v>
       </c>
       <c r="J42">
-        <v>0.407888489208633</v>
+        <v>0.40788848920863302</v>
       </c>
       <c r="K42">
-        <v>0.4428489208633093</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+        <v>0.44284892086330929</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B43">
-        <v>0.4769020771513353</v>
+        <v>0.47690207715133531</v>
       </c>
       <c r="C43">
-        <v>0.3973086053412463</v>
+        <v>0.39730860534124629</v>
       </c>
       <c r="D43">
-        <v>0.5126745796241347</v>
+        <v>0.51267457962413465</v>
       </c>
       <c r="E43">
-        <v>0.554759643916914</v>
+        <v>0.55475964391691401</v>
       </c>
       <c r="F43">
-        <v>0.4331567754698318</v>
+        <v>0.43315677546983178</v>
       </c>
       <c r="G43">
-        <v>0.5138793273986152</v>
+        <v>0.51387932739861519</v>
       </c>
       <c r="H43">
-        <v>0.4739866468842729</v>
+        <v>0.47398664688427289</v>
       </c>
       <c r="I43">
-        <v>0.5604357072205737</v>
+        <v>0.56043570722057368</v>
       </c>
       <c r="J43">
-        <v>0.5184154302670624</v>
+        <v>0.51841543026706238</v>
       </c>
       <c r="K43">
-        <v>0.3225237388724035</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+        <v>0.32252373887240349</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B44">
-        <v>0.5244335260115607</v>
+        <v>0.52443352601156068</v>
       </c>
       <c r="C44">
-        <v>0.5141040462427746</v>
+        <v>0.51410404624277461</v>
       </c>
       <c r="D44">
-        <v>0.5269306358381503</v>
+        <v>0.52693063583815025</v>
       </c>
       <c r="E44">
-        <v>0.5671618497109827</v>
+        <v>0.56716184971098271</v>
       </c>
       <c r="F44">
-        <v>0.5479248554913295</v>
+        <v>0.54792485549132952</v>
       </c>
       <c r="G44">
-        <v>0.535728323699422</v>
+        <v>0.53572832369942203</v>
       </c>
       <c r="H44">
-        <v>0.4914624277456647</v>
+        <v>0.49146242774566468</v>
       </c>
       <c r="I44">
-        <v>0.6546878612716762</v>
+        <v>0.65468786127167622</v>
       </c>
       <c r="J44">
-        <v>0.5156820809248555</v>
+        <v>0.51568208092485546</v>
       </c>
       <c r="K44">
         <v>0.4449421965317919</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B45">
-        <v>0.586478737395879</v>
+        <v>0.58647873739587897</v>
       </c>
       <c r="C45">
-        <v>0.5687277509864095</v>
+        <v>0.56872775098640949</v>
       </c>
       <c r="D45">
-        <v>0.5360118369136345</v>
+        <v>0.53601183691363452</v>
       </c>
       <c r="E45">
-        <v>0.5797818939061815</v>
+        <v>0.57978189390618151</v>
       </c>
       <c r="F45">
-        <v>0.6501733888645331</v>
+        <v>0.65017338886453313</v>
       </c>
       <c r="G45">
-        <v>0.6305447172292853</v>
+        <v>0.63054471722928529</v>
       </c>
       <c r="H45">
-        <v>0.5047825515124945</v>
+        <v>0.50478255151249452</v>
       </c>
       <c r="I45">
-        <v>0.6717356422621659</v>
+        <v>0.67173564226216587</v>
       </c>
       <c r="J45">
-        <v>0.6370848312143796</v>
+        <v>0.63708483121437964</v>
       </c>
       <c r="K45">
         <v>0.5167533976326173</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B46">
-        <v>0.552</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="C46">
-        <v>0.419</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="D46">
         <v>0.66</v>
@@ -2137,22 +2195,22 @@
         <v>0.5</v>
       </c>
       <c r="F46">
-        <v>0.5489999999999999</v>
+        <v>0.54899999999999993</v>
       </c>
       <c r="G46">
         <v>0.375</v>
       </c>
       <c r="H46">
-        <v>0.475</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="I46">
-        <v>0.765</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="J46">
         <v>0.61</v>
       </c>
       <c r="K46">
-        <v>0.5329999999999999</v>
+        <v>0.53299999999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>